<commit_message>
Updated with Action data
</commit_message>
<xml_diff>
--- a/selevance/src/test/resources/data/Action1.xlsx
+++ b/selevance/src/test/resources/data/Action1.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="31">
   <si>
     <t>Name</t>
   </si>
@@ -25,21 +25,9 @@
     <t>Location</t>
   </si>
   <si>
-    <t>HOME</t>
-  </si>
-  <si>
-    <t>com.demo.test.Home</t>
-  </si>
-  <si>
     <t>Action</t>
   </si>
   <si>
-    <t>DoWork1</t>
-  </si>
-  <si>
-    <t>DoWork2</t>
-  </si>
-  <si>
     <t>TestCaseID</t>
   </si>
   <si>
@@ -73,55 +61,55 @@
     <t>TC002</t>
   </si>
   <si>
-    <t>Some thing about test case 2</t>
-  </si>
-  <si>
-    <t>Some thing about test case 1</t>
-  </si>
-  <si>
-    <t>DoWork3</t>
-  </si>
-  <si>
-    <t>DoWork4</t>
-  </si>
-  <si>
-    <t>DoWork5</t>
-  </si>
-  <si>
-    <t>DoWork6</t>
-  </si>
-  <si>
-    <t>DoWork7</t>
-  </si>
-  <si>
-    <t>Sumon</t>
-  </si>
-  <si>
-    <t>Ram</t>
-  </si>
-  <si>
-    <t>TC003</t>
-  </si>
-  <si>
-    <t>PDP</t>
-  </si>
-  <si>
-    <t>com.demo.test.PDP</t>
-  </si>
-  <si>
-    <t>DoPDP1</t>
-  </si>
-  <si>
-    <t>DoPDP2</t>
-  </si>
-  <si>
-    <t>DoPDP3</t>
-  </si>
-  <si>
-    <t>DoPDP4</t>
-  </si>
-  <si>
-    <t>DoPDP5</t>
+    <t>Common</t>
+  </si>
+  <si>
+    <t>verifyCatragory</t>
+  </si>
+  <si>
+    <t>verifyManufacturers</t>
+  </si>
+  <si>
+    <t>verifyInformationSection</t>
+  </si>
+  <si>
+    <t>verifyShopByPrice</t>
+  </si>
+  <si>
+    <t>validateSearch</t>
+  </si>
+  <si>
+    <t>verifyShopByPriceAppearance</t>
+  </si>
+  <si>
+    <t>Home</t>
+  </si>
+  <si>
+    <t>com.tomatocart.business.flow.HomeInfo</t>
+  </si>
+  <si>
+    <t>com.tomatocart.business.flow.CommonInfo</t>
+  </si>
+  <si>
+    <t>verifyFirstProduct</t>
+  </si>
+  <si>
+    <t>searchProduct</t>
+  </si>
+  <si>
+    <t>validateAutoComplete</t>
+  </si>
+  <si>
+    <t>Validate First Product</t>
+  </si>
+  <si>
+    <t>Device</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>Verify Shop By Price Appearance</t>
   </si>
 </sst>
 </file>
@@ -480,46 +468,46 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -529,191 +517,126 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>21</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="2" t="s">
         <v>21</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>6</v>
+        <v>21</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="A14" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="A15" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -723,15 +646,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -742,81 +666,81 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="2" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" s="2" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" s="2" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>24</v>
@@ -824,57 +748,24 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" s="2" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="A11" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -884,10 +775,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -898,46 +789,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated with Test data
</commit_message>
<xml_diff>
--- a/selevance/src/test/resources/data/Action1.xlsx
+++ b/selevance/src/test/resources/data/Action1.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="32">
   <si>
     <t>Name</t>
   </si>
@@ -110,6 +110,9 @@
   </si>
   <si>
     <t>Verify Shop By Price Appearance</t>
+  </si>
+  <si>
+    <t>Samsung</t>
   </si>
 </sst>
 </file>
@@ -775,9 +778,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -814,6 +819,20 @@
         <v>12</v>
       </c>
     </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>